<commit_message>
etape 4 CORR + etape 5 OPTIM
etape 5 ne fonctionne pas encore.
</commit_message>
<xml_diff>
--- a/tests/tests.xlsx
+++ b/tests/tests.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
   <si>
     <t>Etape</t>
   </si>
@@ -129,6 +129,48 @@
   </si>
   <si>
     <t>affiche toutes les fautes quand il y  en a plusieurs</t>
+  </si>
+  <si>
+    <t>4 : checkClass()</t>
+  </si>
+  <si>
+    <t>message erreur + nom + classe fautive (classe anormale et classe attendue) + stop</t>
+  </si>
+  <si>
+    <t>classe incorrecte factor</t>
+  </si>
+  <si>
+    <t>classe incorrecte integer</t>
+  </si>
+  <si>
+    <t>classe incorrecte numeric</t>
+  </si>
+  <si>
+    <t>classe attendue IND</t>
+  </si>
+  <si>
+    <t>classe attendue QUAD</t>
+  </si>
+  <si>
+    <t>factor, integer ou numeric : message info</t>
+  </si>
+  <si>
+    <t>5: checkFactor()</t>
+  </si>
+  <si>
+    <t>uniquement les colonnes de classe factor</t>
+  </si>
+  <si>
+    <t>modalité correspond à l'attendu</t>
+  </si>
+  <si>
+    <t>modalité ne correspond pas à l'attendu</t>
+  </si>
+  <si>
+    <t>message erreur + col/numero/contenu des lignes + contenu attendu</t>
+  </si>
+  <si>
+    <t>message d'information pertinent</t>
   </si>
 </sst>
 </file>
@@ -164,11 +206,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,7 +685,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>30</v>
       </c>
@@ -653,12 +696,94 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>